<commit_message>
change in Data File
</commit_message>
<xml_diff>
--- a/provide/test/TestDataProvide.xlsx
+++ b/provide/test/TestDataProvide.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F864A9E-E42D-4CE9-A71B-8EF94516E045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59AA0E90-6DCD-431D-8AB1-66B7601B23E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -238,6 +238,9 @@
   </si>
   <si>
     <t>EMEAAD\srofidal</t>
+  </si>
+  <si>
+    <t>EMEAAD\pvergez</t>
   </si>
 </sst>
 </file>
@@ -346,7 +349,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -367,6 +370,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -650,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF3" sqref="AF3"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB3" sqref="AB3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +865,7 @@
       <c r="Z2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AA2" s="16" t="s">
         <v>35</v>
       </c>
       <c r="AB2" s="9" t="s">
@@ -959,8 +963,8 @@
       <c r="Z3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="6" t="s">
-        <v>35</v>
+      <c r="AA3" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="AB3" s="9" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
testing 3 entity 362,010 and 413
</commit_message>
<xml_diff>
--- a/provide/test/TestDataProvide.xlsx
+++ b/provide/test/TestDataProvide.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584CF26D-6D6D-4709-84F9-532A4A2FE999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60101181-0950-483B-8C0F-FCD395787DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5385" yWindow="3615" windowWidth="21600" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="79">
   <si>
     <t>OrderDesc</t>
   </si>
@@ -189,24 +189,12 @@
     <t>yes</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>SW &amp; Solutions - IS-HR</t>
-  </si>
-  <si>
-    <t>SAAS FIXED COST</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
     <t>99</t>
   </si>
   <si>
-    <t>EMEAAD\lbaisin</t>
-  </si>
-  <si>
     <t>413</t>
   </si>
   <si>
@@ -216,9 +204,6 @@
     <t>Product4</t>
   </si>
   <si>
-    <t>[DSI-BUILD]-OAR-TEST CASE 8</t>
-  </si>
-  <si>
     <t>Services - Hosting</t>
   </si>
   <si>
@@ -228,9 +213,6 @@
     <t>50000</t>
   </si>
   <si>
-    <t>100000</t>
-  </si>
-  <si>
     <t>TND</t>
   </si>
   <si>
@@ -247,13 +229,85 @@
   </si>
   <si>
     <t>S00014700001</t>
+  </si>
+  <si>
+    <t>EMEAAD\anchaudhary</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>Test Automation India Anmol</t>
+  </si>
+  <si>
+    <t>Product2</t>
+  </si>
+  <si>
+    <t>HW - Network Security</t>
+  </si>
+  <si>
+    <t>S00008044001</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>MAINT FIXED COST</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>EMEAAD\pvergez</t>
+  </si>
+  <si>
+    <t>362</t>
+  </si>
+  <si>
+    <t>[DSI-BUILD]-OAR-TEST CASE 5</t>
+  </si>
+  <si>
+    <t>Product1</t>
+  </si>
+  <si>
+    <t>HW - Screen for PC</t>
+  </si>
+  <si>
+    <t>S00001610001</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>5000</t>
+  </si>
+  <si>
+    <t>Eur</t>
+  </si>
+  <si>
+    <t>RENT FIXED COST</t>
+  </si>
+  <si>
+    <t>EMEAAD\srofidal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -305,6 +359,18 @@
       <color rgb="FF202124"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
+      <name val="Fira Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -364,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -383,6 +449,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -664,10 +756,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG3"/>
+  <dimension ref="A1:AG4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1:AJ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,46 +901,46 @@
         <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>36</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>35</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="Q2" s="12" t="s">
         <v>32</v>
@@ -863,13 +955,13 @@
         <v>32</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="W2" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="X2" s="10"/>
       <c r="Y2" s="10" t="s">
@@ -889,111 +981,212 @@
         <v>32</v>
       </c>
       <c r="AE2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="AF2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG2" s="6" t="s">
+      <c r="H3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="N3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="R3" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="T3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="U3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="V3" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="W3" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="X3" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y3" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB3" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD3" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE3" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG3" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="6" t="s">
+      <c r="C4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E4" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="33" t="s">
+        <v>73</v>
+      </c>
+      <c r="K4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="M4" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="P4" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="Q4" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="R4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="U4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="V4" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="R3" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="V3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="W3" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="X3" s="10"/>
-      <c r="Y3" s="10" t="s">
+      <c r="X4" s="31"/>
+      <c r="Y4" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="Z3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB3" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG3" s="6" t="s">
+      <c r="Z4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB4" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC4" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD4" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE4" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="AF4" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="AG4" s="32" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1001,13 +1194,14 @@
   <phoneticPr fontId="6" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{C1B78C7E-7911-43ED-AF99-9E56177BCD8F}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{2C31F390-2496-4C99-ACCD-55C7E6D3A1AC}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{08A1F94F-D207-4E1B-A1F4-653E7269FE7D}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;1#&amp;"Tahoma"&amp;9&amp;KCF022BC2 - Restricted</oddFooter>
   </headerFooter>
-  <legacyDrawing r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>